<commit_message>
Correct some mistakes in the BPSFH dataset
</commit_message>
<xml_diff>
--- a/harana/datasets/BPSFH/26/chords.xlsx
+++ b/harana/datasets/BPSFH/26/chords.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iis519\Desktop\Dataset\BPS Dataset\26\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qiaoyu/Desktop/video_music/harana/harana/datasets/BPSFH/26/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71761A5-2E0C-5247-967C-9920B37000BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12396"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1049,19 +1050,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -1125,7 +1126,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1136,9 +1137,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1158,7 +1156,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1435,19 +1433,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O393"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="7" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -1470,7 +1468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1493,7 +1491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1516,7 +1514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -1539,7 +1537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -1562,7 +1560,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5.5</v>
       </c>
@@ -1585,7 +1583,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1608,7 +1606,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6.5</v>
       </c>
@@ -1631,7 +1629,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1654,7 +1652,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1677,7 +1675,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>8.5</v>
       </c>
@@ -1700,7 +1698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1723,7 +1721,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9.5</v>
       </c>
@@ -1746,7 +1744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1769,7 +1767,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>10.5</v>
       </c>
@@ -1792,7 +1790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -1815,7 +1813,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>11.5</v>
       </c>
@@ -1838,7 +1836,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>12</v>
       </c>
@@ -1861,7 +1859,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>13</v>
       </c>
@@ -1884,7 +1882,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>14</v>
       </c>
@@ -1907,7 +1905,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -1930,7 +1928,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>17</v>
       </c>
@@ -1953,7 +1951,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>17.5</v>
       </c>
@@ -1976,7 +1974,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>18</v>
       </c>
@@ -1999,7 +1997,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>19</v>
       </c>
@@ -2022,7 +2020,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>19.5</v>
       </c>
@@ -2045,7 +2043,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>20</v>
       </c>
@@ -2068,7 +2066,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>20.5</v>
       </c>
@@ -2091,7 +2089,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>21</v>
       </c>
@@ -2114,7 +2112,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>21.5</v>
       </c>
@@ -2137,7 +2135,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>22</v>
       </c>
@@ -2160,7 +2158,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>23.5</v>
       </c>
@@ -2183,7 +2181,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>24</v>
       </c>
@@ -2206,7 +2204,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>25.5</v>
       </c>
@@ -2229,7 +2227,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>26</v>
       </c>
@@ -2252,7 +2250,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>27.5</v>
       </c>
@@ -2275,7 +2273,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>27.75</v>
       </c>
@@ -2298,7 +2296,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>29.25</v>
       </c>
@@ -2321,7 +2319,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>29.5</v>
       </c>
@@ -2344,7 +2342,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>29.75</v>
       </c>
@@ -2367,35 +2365,35 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
         <v>32</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B41" s="1">
         <v>35</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="1">
         <v>4</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="E41" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="4">
-        <v>1</v>
-      </c>
-      <c r="G41" s="4" t="s">
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>134</v>
       </c>
       <c r="K41" s="1"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>35</v>
       </c>
@@ -2423,7 +2421,7 @@
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>36</v>
       </c>
@@ -2451,7 +2449,7 @@
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>37</v>
       </c>
@@ -2479,7 +2477,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>38</v>
       </c>
@@ -2507,7 +2505,7 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>39</v>
       </c>
@@ -2535,7 +2533,7 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>40</v>
       </c>
@@ -2563,7 +2561,7 @@
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43</v>
       </c>
@@ -2591,7 +2589,7 @@
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>44</v>
       </c>
@@ -2619,7 +2617,7 @@
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>45</v>
       </c>
@@ -2647,7 +2645,7 @@
       <c r="N50" s="1"/>
       <c r="O50" s="1"/>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>46</v>
       </c>
@@ -2675,7 +2673,7 @@
       <c r="N51" s="1"/>
       <c r="O51" s="1"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -2703,7 +2701,7 @@
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2731,7 +2729,7 @@
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>56</v>
       </c>
@@ -2759,7 +2757,7 @@
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>60</v>
       </c>
@@ -2787,7 +2785,7 @@
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>62</v>
       </c>
@@ -2815,7 +2813,7 @@
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>64</v>
       </c>
@@ -2843,7 +2841,7 @@
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>68</v>
       </c>
@@ -2871,7 +2869,7 @@
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>72</v>
       </c>
@@ -2899,7 +2897,7 @@
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>76</v>
       </c>
@@ -2927,7 +2925,7 @@
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>78</v>
       </c>
@@ -2955,7 +2953,7 @@
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>80</v>
       </c>
@@ -2983,7 +2981,7 @@
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>84</v>
       </c>
@@ -3011,7 +3009,7 @@
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>88</v>
       </c>
@@ -3039,7 +3037,7 @@
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>96</v>
       </c>
@@ -3067,7 +3065,7 @@
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>98</v>
       </c>
@@ -3095,7 +3093,7 @@
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>100</v>
       </c>
@@ -3123,7 +3121,7 @@
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>102</v>
       </c>
@@ -3151,7 +3149,7 @@
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>104</v>
       </c>
@@ -3179,7 +3177,7 @@
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>108</v>
       </c>
@@ -3207,7 +3205,7 @@
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>112</v>
       </c>
@@ -3235,7 +3233,7 @@
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>116</v>
       </c>
@@ -3263,7 +3261,7 @@
       <c r="N72" s="1"/>
       <c r="O72" s="1"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>120</v>
       </c>
@@ -3291,7 +3289,7 @@
       <c r="N73" s="1"/>
       <c r="O73" s="1"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>124</v>
       </c>
@@ -3319,7 +3317,7 @@
       <c r="N74" s="1"/>
       <c r="O74" s="1"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>128</v>
       </c>
@@ -3347,7 +3345,7 @@
       <c r="N75" s="1"/>
       <c r="O75" s="1"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>130</v>
       </c>
@@ -3375,7 +3373,7 @@
       <c r="N76" s="1"/>
       <c r="O76" s="1"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>132</v>
       </c>
@@ -3403,7 +3401,7 @@
       <c r="N77" s="1"/>
       <c r="O77" s="1"/>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>134</v>
       </c>
@@ -3431,7 +3429,7 @@
       <c r="N78" s="1"/>
       <c r="O78" s="1"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>136</v>
       </c>
@@ -3459,7 +3457,7 @@
       <c r="N79" s="1"/>
       <c r="O79" s="1"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>140</v>
       </c>
@@ -3487,7 +3485,7 @@
       <c r="N80" s="1"/>
       <c r="O80" s="1"/>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>144</v>
       </c>
@@ -3515,7 +3513,7 @@
       <c r="N81" s="1"/>
       <c r="O81" s="1"/>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>146</v>
       </c>
@@ -3543,7 +3541,7 @@
       <c r="N82" s="1"/>
       <c r="O82" s="1"/>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>148</v>
       </c>
@@ -3571,7 +3569,7 @@
       <c r="N83" s="1"/>
       <c r="O83" s="1"/>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>164</v>
       </c>
@@ -3599,7 +3597,7 @@
       <c r="N84" s="1"/>
       <c r="O84" s="1"/>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>165</v>
       </c>
@@ -3627,7 +3625,7 @@
       <c r="N85" s="1"/>
       <c r="O85" s="1"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>167</v>
       </c>
@@ -3655,7 +3653,7 @@
       <c r="N86" s="1"/>
       <c r="O86" s="1"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>169</v>
       </c>
@@ -3683,7 +3681,7 @@
       <c r="N87" s="1"/>
       <c r="O87" s="1"/>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>171</v>
       </c>
@@ -3711,7 +3709,7 @@
       <c r="N88" s="1"/>
       <c r="O88" s="1"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>174</v>
       </c>
@@ -3739,7 +3737,7 @@
       <c r="N89" s="1"/>
       <c r="O89" s="1"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>175</v>
       </c>
@@ -3767,7 +3765,7 @@
       <c r="N90" s="1"/>
       <c r="O90" s="1"/>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>176</v>
       </c>
@@ -3795,7 +3793,7 @@
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>177</v>
       </c>
@@ -3823,7 +3821,7 @@
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>178</v>
       </c>
@@ -3851,7 +3849,7 @@
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>179</v>
       </c>
@@ -3879,7 +3877,7 @@
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>180</v>
       </c>
@@ -3907,7 +3905,7 @@
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>181</v>
       </c>
@@ -3935,7 +3933,7 @@
       <c r="N96" s="1"/>
       <c r="O96" s="1"/>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>183</v>
       </c>
@@ -3963,7 +3961,7 @@
       <c r="N97" s="1"/>
       <c r="O97" s="1"/>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>185</v>
       </c>
@@ -3991,7 +3989,7 @@
       <c r="N98" s="1"/>
       <c r="O98" s="1"/>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>187</v>
       </c>
@@ -4019,7 +4017,7 @@
       <c r="N99" s="1"/>
       <c r="O99" s="1"/>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>190</v>
       </c>
@@ -4047,7 +4045,7 @@
       <c r="N100" s="1"/>
       <c r="O100" s="1"/>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>191</v>
       </c>
@@ -4075,7 +4073,7 @@
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>192</v>
       </c>
@@ -4103,7 +4101,7 @@
       <c r="N102" s="1"/>
       <c r="O102" s="1"/>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>193</v>
       </c>
@@ -4131,7 +4129,7 @@
       <c r="N103" s="1"/>
       <c r="O103" s="1"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>194</v>
       </c>
@@ -4159,7 +4157,7 @@
       <c r="N104" s="1"/>
       <c r="O104" s="1"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>195</v>
       </c>
@@ -4187,7 +4185,7 @@
       <c r="N105" s="1"/>
       <c r="O105" s="1"/>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>196</v>
       </c>
@@ -4215,7 +4213,7 @@
       <c r="N106" s="1"/>
       <c r="O106" s="1"/>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>200</v>
       </c>
@@ -4243,7 +4241,7 @@
       <c r="N107" s="1"/>
       <c r="O107" s="1"/>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>204</v>
       </c>
@@ -4271,7 +4269,7 @@
       <c r="N108" s="1"/>
       <c r="O108" s="1"/>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>208</v>
       </c>
@@ -4299,7 +4297,7 @@
       <c r="N109" s="1"/>
       <c r="O109" s="1"/>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>212</v>
       </c>
@@ -4327,7 +4325,7 @@
       <c r="N110" s="1"/>
       <c r="O110" s="1"/>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>228</v>
       </c>
@@ -4355,7 +4353,7 @@
       <c r="N111" s="1"/>
       <c r="O111" s="1"/>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>232</v>
       </c>
@@ -4383,7 +4381,7 @@
       <c r="N112" s="1"/>
       <c r="O112" s="1"/>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>236</v>
       </c>
@@ -4411,26 +4409,26 @@
       <c r="N113" s="1"/>
       <c r="O113" s="1"/>
     </row>
-    <row r="114" spans="1:15" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="5">
+    <row r="114" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="4">
         <v>240</v>
       </c>
-      <c r="B114" s="5">
+      <c r="B114" s="4">
         <v>244</v>
       </c>
-      <c r="C114" s="5" t="s">
+      <c r="C114" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D114" s="6" t="s">
+      <c r="D114" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E114" s="5" t="s">
+      <c r="E114" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F114" s="5">
+      <c r="F114" s="4">
         <v>3</v>
       </c>
-      <c r="G114" s="5" t="s">
+      <c r="G114" s="4" t="s">
         <v>133</v>
       </c>
       <c r="K114" s="1"/>
@@ -4439,7 +4437,7 @@
       <c r="N114" s="1"/>
       <c r="O114" s="1"/>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>244</v>
       </c>
@@ -4449,20 +4447,20 @@
       <c r="C115" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D115" s="4">
+      <c r="D115" s="1">
         <v>4</v>
       </c>
-      <c r="E115" s="4" t="s">
+      <c r="E115" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F115" s="4">
-        <v>1</v>
-      </c>
-      <c r="G115" s="4" t="s">
+      <c r="F115" s="1">
+        <v>1</v>
+      </c>
+      <c r="G115" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>247</v>
       </c>
@@ -4485,7 +4483,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>248</v>
       </c>
@@ -4508,7 +4506,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>249</v>
       </c>
@@ -4531,7 +4529,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>250</v>
       </c>
@@ -4554,7 +4552,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>251</v>
       </c>
@@ -4577,7 +4575,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>252</v>
       </c>
@@ -4600,7 +4598,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>255</v>
       </c>
@@ -4623,7 +4621,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>256</v>
       </c>
@@ -4646,7 +4644,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>257</v>
       </c>
@@ -4669,7 +4667,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>258</v>
       </c>
@@ -4692,7 +4690,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>260</v>
       </c>
@@ -4715,7 +4713,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>264</v>
       </c>
@@ -4738,7 +4736,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>268</v>
       </c>
@@ -4761,7 +4759,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>272</v>
       </c>
@@ -4784,7 +4782,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>274</v>
       </c>
@@ -4807,7 +4805,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>276</v>
       </c>
@@ -4830,7 +4828,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>280</v>
       </c>
@@ -4853,7 +4851,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>284</v>
       </c>
@@ -4876,7 +4874,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>288</v>
       </c>
@@ -4899,7 +4897,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>290</v>
       </c>
@@ -4922,7 +4920,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>292</v>
       </c>
@@ -4945,7 +4943,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>296</v>
       </c>
@@ -4968,7 +4966,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>300</v>
       </c>
@@ -4991,7 +4989,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>308</v>
       </c>
@@ -5014,7 +5012,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>310</v>
       </c>
@@ -5037,7 +5035,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>312</v>
       </c>
@@ -5060,7 +5058,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>314</v>
       </c>
@@ -5083,7 +5081,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>316</v>
       </c>
@@ -5106,7 +5104,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>320</v>
       </c>
@@ -5129,7 +5127,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>324</v>
       </c>
@@ -5152,7 +5150,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>328</v>
       </c>
@@ -5175,7 +5173,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>332</v>
       </c>
@@ -5198,7 +5196,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>336</v>
       </c>
@@ -5221,7 +5219,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>340</v>
       </c>
@@ -5244,7 +5242,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>342</v>
       </c>
@@ -5267,7 +5265,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>344</v>
       </c>
@@ -5290,7 +5288,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>346</v>
       </c>
@@ -5313,7 +5311,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>348</v>
       </c>
@@ -5336,7 +5334,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>352</v>
       </c>
@@ -5359,7 +5357,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>356</v>
       </c>
@@ -5382,7 +5380,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>358</v>
       </c>
@@ -5405,7 +5403,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>360</v>
       </c>
@@ -5428,7 +5426,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>376</v>
       </c>
@@ -5451,7 +5449,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>377</v>
       </c>
@@ -5474,7 +5472,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>379</v>
       </c>
@@ -5497,7 +5495,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>381</v>
       </c>
@@ -5520,7 +5518,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>383</v>
       </c>
@@ -5543,7 +5541,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>386</v>
       </c>
@@ -5566,7 +5564,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>387</v>
       </c>
@@ -5589,7 +5587,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>388</v>
       </c>
@@ -5612,7 +5610,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>389</v>
       </c>
@@ -5635,7 +5633,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>390</v>
       </c>
@@ -5658,7 +5656,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>391</v>
       </c>
@@ -5681,7 +5679,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>392</v>
       </c>
@@ -5704,7 +5702,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>393</v>
       </c>
@@ -5727,7 +5725,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>395</v>
       </c>
@@ -5750,7 +5748,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>397</v>
       </c>
@@ -5773,7 +5771,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>399</v>
       </c>
@@ -5796,7 +5794,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>402</v>
       </c>
@@ -5819,7 +5817,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>403</v>
       </c>
@@ -5842,7 +5840,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>404</v>
       </c>
@@ -5865,7 +5863,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>405</v>
       </c>
@@ -5888,7 +5886,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>406</v>
       </c>
@@ -5911,7 +5909,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>407</v>
       </c>
@@ -5934,7 +5932,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>408</v>
       </c>
@@ -5957,7 +5955,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>412</v>
       </c>
@@ -5980,7 +5978,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>416</v>
       </c>
@@ -6003,7 +6001,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>420</v>
       </c>
@@ -6026,7 +6024,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>424</v>
       </c>
@@ -6049,7 +6047,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>440</v>
       </c>
@@ -6072,7 +6070,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>444</v>
       </c>
@@ -6095,7 +6093,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>448</v>
       </c>
@@ -6118,30 +6116,30 @@
         <v>79</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A188" s="7">
+    <row r="188" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="6">
         <v>452</v>
       </c>
-      <c r="B188" s="7">
+      <c r="B188" s="6">
         <v>456</v>
       </c>
-      <c r="C188" s="8" t="s">
+      <c r="C188" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="D188" s="8">
+      <c r="D188" s="7">
         <v>6</v>
       </c>
-      <c r="E188" s="8" t="s">
+      <c r="E188" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="F188" s="8">
-        <v>1</v>
-      </c>
-      <c r="G188" s="8" t="s">
+      <c r="F188" s="7">
+        <v>1</v>
+      </c>
+      <c r="G188" s="7" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>456</v>
       </c>
@@ -6164,7 +6162,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>458</v>
       </c>
@@ -6187,7 +6185,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>460</v>
       </c>
@@ -6210,7 +6208,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>462</v>
       </c>
@@ -6233,7 +6231,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>464</v>
       </c>
@@ -6256,7 +6254,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>465</v>
       </c>
@@ -6279,7 +6277,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>466</v>
       </c>
@@ -6302,7 +6300,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>467</v>
       </c>
@@ -6325,7 +6323,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>476</v>
       </c>
@@ -6348,7 +6346,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>480</v>
       </c>
@@ -6371,7 +6369,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>483</v>
       </c>
@@ -6394,7 +6392,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>492</v>
       </c>
@@ -6417,7 +6415,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>508</v>
       </c>
@@ -6440,7 +6438,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>524</v>
       </c>
@@ -6463,7 +6461,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>540</v>
       </c>
@@ -6486,7 +6484,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>543</v>
       </c>
@@ -6509,7 +6507,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>544</v>
       </c>
@@ -6532,7 +6530,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>545</v>
       </c>
@@ -6555,7 +6553,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>546</v>
       </c>
@@ -6578,7 +6576,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>547</v>
       </c>
@@ -6601,7 +6599,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>548</v>
       </c>
@@ -6624,7 +6622,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>549</v>
       </c>
@@ -6647,7 +6645,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>550</v>
       </c>
@@ -6670,7 +6668,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>551</v>
       </c>
@@ -6693,7 +6691,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>552</v>
       </c>
@@ -6716,7 +6714,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>556</v>
       </c>
@@ -6739,7 +6737,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>564</v>
       </c>
@@ -6762,7 +6760,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>568</v>
       </c>
@@ -6785,7 +6783,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>572</v>
       </c>
@@ -6808,7 +6806,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>576</v>
       </c>
@@ -6831,7 +6829,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>580</v>
       </c>
@@ -6854,7 +6852,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>584</v>
       </c>
@@ -6877,7 +6875,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>588</v>
       </c>
@@ -6900,7 +6898,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>596</v>
       </c>
@@ -6923,30 +6921,30 @@
         <v>188</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A223" s="9">
+    <row r="223" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="8">
         <v>600</v>
       </c>
-      <c r="B223" s="9">
+      <c r="B223" s="8">
         <v>618</v>
       </c>
-      <c r="C223" s="9" t="s">
+      <c r="C223" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D223" s="9">
+      <c r="D223" s="8">
         <v>4</v>
       </c>
-      <c r="E223" s="9" t="s">
+      <c r="E223" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="F223" s="9">
-        <v>1</v>
-      </c>
-      <c r="G223" s="9" t="s">
+      <c r="F223" s="8">
+        <v>1</v>
+      </c>
+      <c r="G223" s="8" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>618</v>
       </c>
@@ -6969,7 +6967,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>620</v>
       </c>
@@ -6992,7 +6990,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>621</v>
       </c>
@@ -7015,7 +7013,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>622</v>
       </c>
@@ -7038,7 +7036,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>623</v>
       </c>
@@ -7061,7 +7059,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>624</v>
       </c>
@@ -7084,7 +7082,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>627</v>
       </c>
@@ -7107,7 +7105,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>628</v>
       </c>
@@ -7130,7 +7128,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>629</v>
       </c>
@@ -7153,7 +7151,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>630</v>
       </c>
@@ -7176,7 +7174,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>632</v>
       </c>
@@ -7199,7 +7197,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>636</v>
       </c>
@@ -7222,7 +7220,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>640</v>
       </c>
@@ -7245,7 +7243,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>644</v>
       </c>
@@ -7268,7 +7266,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>646</v>
       </c>
@@ -7291,7 +7289,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>648</v>
       </c>
@@ -7314,7 +7312,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>650</v>
       </c>
@@ -7337,7 +7335,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>652</v>
       </c>
@@ -7360,7 +7358,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>660</v>
       </c>
@@ -7383,7 +7381,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>662</v>
       </c>
@@ -7406,7 +7404,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>664</v>
       </c>
@@ -7429,7 +7427,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>668</v>
       </c>
@@ -7452,7 +7450,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>672</v>
       </c>
@@ -7475,7 +7473,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>676</v>
       </c>
@@ -7498,7 +7496,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>678</v>
       </c>
@@ -7521,7 +7519,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>680</v>
       </c>
@@ -7544,7 +7542,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>682</v>
       </c>
@@ -7567,7 +7565,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>684</v>
       </c>
@@ -7590,7 +7588,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>688</v>
       </c>
@@ -7613,7 +7611,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>692</v>
       </c>
@@ -7636,7 +7634,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>696</v>
       </c>
@@ -7659,7 +7657,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>700</v>
       </c>
@@ -7682,7 +7680,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>704</v>
       </c>
@@ -7705,7 +7703,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>708</v>
       </c>
@@ -7728,7 +7726,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>710</v>
       </c>
@@ -7751,7 +7749,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>712</v>
       </c>
@@ -7774,7 +7772,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>714</v>
       </c>
@@ -7797,7 +7795,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>716</v>
       </c>
@@ -7820,7 +7818,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>720</v>
       </c>
@@ -7843,7 +7841,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="263" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>724</v>
       </c>
@@ -7866,7 +7864,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>726</v>
       </c>
@@ -7889,7 +7887,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>728</v>
       </c>
@@ -7912,7 +7910,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>744</v>
       </c>
@@ -7935,7 +7933,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>745</v>
       </c>
@@ -7958,7 +7956,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>747</v>
       </c>
@@ -7981,7 +7979,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="269" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>749</v>
       </c>
@@ -8004,7 +8002,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="270" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>751</v>
       </c>
@@ -8027,7 +8025,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="271" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>754</v>
       </c>
@@ -8050,7 +8048,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="272" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>755</v>
       </c>
@@ -8073,7 +8071,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>756</v>
       </c>
@@ -8096,7 +8094,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>757</v>
       </c>
@@ -8119,7 +8117,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>758</v>
       </c>
@@ -8142,7 +8140,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>759</v>
       </c>
@@ -8165,7 +8163,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>760</v>
       </c>
@@ -8188,7 +8186,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>761</v>
       </c>
@@ -8211,7 +8209,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>763</v>
       </c>
@@ -8234,7 +8232,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>765</v>
       </c>
@@ -8257,7 +8255,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>767</v>
       </c>
@@ -8280,7 +8278,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>770</v>
       </c>
@@ -8303,7 +8301,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>771</v>
       </c>
@@ -8326,7 +8324,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>772</v>
       </c>
@@ -8349,7 +8347,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>773</v>
       </c>
@@ -8372,7 +8370,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>774</v>
       </c>
@@ -8395,7 +8393,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>775</v>
       </c>
@@ -8418,7 +8416,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>776</v>
       </c>
@@ -8441,7 +8439,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="289" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>780</v>
       </c>
@@ -8464,7 +8462,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="290" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>784</v>
       </c>
@@ -8487,7 +8485,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="291" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>788</v>
       </c>
@@ -8510,7 +8508,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="292" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>792</v>
       </c>
@@ -8533,7 +8531,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="293" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>808</v>
       </c>
@@ -8556,7 +8554,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="294" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>812</v>
       </c>
@@ -8579,7 +8577,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="295" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>816</v>
       </c>
@@ -8602,7 +8600,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="296" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>820</v>
       </c>
@@ -8625,7 +8623,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="297" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>824</v>
       </c>
@@ -8648,7 +8646,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="298" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>827</v>
       </c>
@@ -8671,7 +8669,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="299" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>828</v>
       </c>
@@ -8694,7 +8692,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="300" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>830</v>
       </c>
@@ -8717,7 +8715,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="301" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>832</v>
       </c>
@@ -8740,7 +8738,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="302" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>834</v>
       </c>
@@ -8763,7 +8761,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="303" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>835</v>
       </c>
@@ -8786,7 +8784,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="304" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>836</v>
       </c>
@@ -8809,7 +8807,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="305" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>839</v>
       </c>
@@ -8832,7 +8830,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="306" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>840</v>
       </c>
@@ -8855,7 +8853,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="307" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>841</v>
       </c>
@@ -8878,7 +8876,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="308" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>842</v>
       </c>
@@ -8901,7 +8899,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="309" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>844</v>
       </c>
@@ -8924,7 +8922,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="310" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>848</v>
       </c>
@@ -8947,7 +8945,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="311" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>852</v>
       </c>
@@ -8970,7 +8968,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="312" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>856</v>
       </c>
@@ -8993,7 +8991,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="313" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>858</v>
       </c>
@@ -9016,7 +9014,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="314" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>860</v>
       </c>
@@ -9039,7 +9037,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="315" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>864</v>
       </c>
@@ -9062,7 +9060,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="316" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>868</v>
       </c>
@@ -9085,7 +9083,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="317" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>870</v>
       </c>
@@ -9108,7 +9106,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="318" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>872</v>
       </c>
@@ -9131,7 +9129,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="319" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>876</v>
       </c>
@@ -9154,7 +9152,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="320" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>880</v>
       </c>
@@ -9177,7 +9175,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="321" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>884</v>
       </c>
@@ -9200,7 +9198,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="322" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>888</v>
       </c>
@@ -9223,7 +9221,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="323" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>890</v>
       </c>
@@ -9246,7 +9244,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="324" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>892</v>
       </c>
@@ -9269,7 +9267,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>894</v>
       </c>
@@ -9292,7 +9290,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>896</v>
       </c>
@@ -9315,7 +9313,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="327" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>898</v>
       </c>
@@ -9338,7 +9336,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>908</v>
       </c>
@@ -9361,7 +9359,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>916</v>
       </c>
@@ -9384,7 +9382,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>932</v>
       </c>
@@ -9407,7 +9405,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>940</v>
       </c>
@@ -9430,7 +9428,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>944</v>
       </c>
@@ -9453,7 +9451,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>948</v>
       </c>
@@ -9476,7 +9474,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="334" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>952</v>
       </c>
@@ -9499,7 +9497,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>956</v>
       </c>
@@ -9522,7 +9520,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>960</v>
       </c>
@@ -9545,7 +9543,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="337" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>964</v>
       </c>
@@ -9568,7 +9566,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>968</v>
       </c>
@@ -9591,7 +9589,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>972</v>
       </c>
@@ -9614,7 +9612,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>976</v>
       </c>
@@ -9637,7 +9635,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>980</v>
       </c>
@@ -9660,7 +9658,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
         <v>984</v>
       </c>
@@ -9683,7 +9681,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A343" s="1">
         <v>988</v>
       </c>
@@ -9706,7 +9704,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="344" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A344" s="1">
         <v>992</v>
       </c>
@@ -9729,7 +9727,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A345" s="1">
         <v>996</v>
       </c>
@@ -9752,7 +9750,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="346" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A346" s="1">
         <v>1000</v>
       </c>
@@ -9775,7 +9773,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
         <v>1002</v>
       </c>
@@ -9798,7 +9796,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
         <v>1004</v>
       </c>
@@ -9821,7 +9819,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>1006</v>
       </c>
@@ -9844,7 +9842,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>1008</v>
       </c>
@@ -9867,7 +9865,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>1012</v>
       </c>
@@ -9890,7 +9888,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="352" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>1016</v>
       </c>
@@ -9913,7 +9911,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="353" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>1020</v>
       </c>
@@ -9936,7 +9934,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="354" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>1024</v>
       </c>
@@ -9959,7 +9957,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="355" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>1028</v>
       </c>
@@ -9982,7 +9980,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="356" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>1032</v>
       </c>
@@ -10005,7 +10003,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="357" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>1036</v>
       </c>
@@ -10028,7 +10026,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="358" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>1040</v>
       </c>
@@ -10051,7 +10049,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="359" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>1044</v>
       </c>
@@ -10074,7 +10072,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="360" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>1048</v>
       </c>
@@ -10097,7 +10095,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="361" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>1050</v>
       </c>
@@ -10120,7 +10118,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="362" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>1052</v>
       </c>
@@ -10143,7 +10141,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="363" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
         <v>1053</v>
       </c>
@@ -10166,7 +10164,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="364" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
         <v>1056</v>
       </c>
@@ -10189,7 +10187,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="365" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>1058</v>
       </c>
@@ -10212,7 +10210,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="366" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>1060</v>
       </c>
@@ -10235,7 +10233,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="367" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A367" s="1">
         <v>1061</v>
       </c>
@@ -10258,7 +10256,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="368" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>1064</v>
       </c>
@@ -10281,7 +10279,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="369" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>1068</v>
       </c>
@@ -10304,7 +10302,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="370" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>1084</v>
       </c>
@@ -10327,7 +10325,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="371" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>1088</v>
       </c>
@@ -10350,7 +10348,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="372" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>1092</v>
       </c>
@@ -10373,7 +10371,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="373" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A373" s="1">
         <v>1096</v>
       </c>
@@ -10396,7 +10394,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="374" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A374" s="1">
         <v>1116</v>
       </c>
@@ -10419,7 +10417,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="375" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>1132</v>
       </c>
@@ -10442,7 +10440,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="376" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>1134</v>
       </c>
@@ -10465,7 +10463,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="377" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>1136</v>
       </c>
@@ -10488,7 +10486,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="378" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>1138</v>
       </c>
@@ -10511,7 +10509,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="379" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A379" s="1">
         <v>1140</v>
       </c>
@@ -10534,7 +10532,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="380" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
         <v>1142</v>
       </c>
@@ -10557,7 +10555,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="381" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
         <v>1144</v>
       </c>
@@ -10580,7 +10578,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="382" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A382" s="1">
         <v>1148</v>
       </c>
@@ -10603,7 +10601,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="383" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A383" s="1">
         <v>1152</v>
       </c>
@@ -10626,7 +10624,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="384" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>1156</v>
       </c>
@@ -10649,7 +10647,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="385" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A385" s="1">
         <v>1160</v>
       </c>
@@ -10672,7 +10670,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="386" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A386" s="1">
         <v>1164</v>
       </c>
@@ -10695,7 +10693,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="387" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A387" s="1">
         <v>1168</v>
       </c>
@@ -10718,7 +10716,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="388" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A388" s="1">
         <v>1172</v>
       </c>
@@ -10741,7 +10739,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="389" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A389" s="1">
         <v>1176</v>
       </c>
@@ -10764,7 +10762,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="390" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A390" s="1">
         <v>1180</v>
       </c>
@@ -10787,7 +10785,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="391" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A391" s="1">
         <v>1184</v>
       </c>
@@ -10810,7 +10808,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="392" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A392" s="1">
         <v>1192</v>
       </c>
@@ -10833,7 +10831,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="393" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A393" s="1">
         <v>1196</v>
       </c>

</xml_diff>